<commit_message>
Added model with possible removal of some variables code and results
</commit_message>
<xml_diff>
--- a/Data/EconomicData/MonthlyCPI-BLS.xlsx
+++ b/Data/EconomicData/MonthlyCPI-BLS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\OneDrive\Documents\CodingProjectsStuff\2023SummerResearch-Inflation\COVID-Inflation\Data\EconomicData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE1C9BF-EC3A-418B-AD29-F7602765FB4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{645E57D2-A3B3-4668-98E6-F31C75CEA1DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28665" yWindow="-135" windowWidth="29070" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BLS Data Series" sheetId="1" r:id="rId1"/>
@@ -41,10 +41,10 @@
     <t>MoM-Inflation</t>
   </si>
   <si>
-    <t>Annualized-Inflation</t>
+    <t>Date</t>
   </si>
   <si>
-    <t>Date</t>
+    <t>MoM-Annualized-Inflation</t>
   </si>
 </sst>
 </file>
@@ -111,7 +111,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -127,9 +127,6 @@
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2223,7 +2220,7 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Annualized-Inflation</c:v>
+                  <c:v>MoM-Annualized-Inflation</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>12.37113402</c:v>
@@ -5329,16 +5326,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>54292</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>506729</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>155255</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>480060</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>26670</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5666,8 +5663,8 @@
   <dimension ref="A1:D403"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5680,7 +5677,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -5689,11 +5686,11 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6">
+      <c r="A2" s="4">
         <v>32843</v>
       </c>
       <c r="B2" s="2">
@@ -8968,7 +8965,7 @@
       <c r="A207" s="5">
         <v>39083</v>
       </c>
-      <c r="B207" s="7">
+      <c r="B207" s="6">
         <v>202.416</v>
       </c>
       <c r="C207">
@@ -8984,7 +8981,7 @@
       <c r="A208" s="5">
         <v>39114</v>
       </c>
-      <c r="B208" s="7">
+      <c r="B208" s="6">
         <v>203.499</v>
       </c>
       <c r="C208">
@@ -9000,7 +8997,7 @@
       <c r="A209" s="5">
         <v>39142</v>
       </c>
-      <c r="B209" s="7">
+      <c r="B209" s="6">
         <v>205.352</v>
       </c>
       <c r="C209">
@@ -9016,7 +9013,7 @@
       <c r="A210" s="5">
         <v>39173</v>
       </c>
-      <c r="B210" s="7">
+      <c r="B210" s="6">
         <v>206.68600000000001</v>
       </c>
       <c r="C210">
@@ -9032,7 +9029,7 @@
       <c r="A211" s="5">
         <v>39203</v>
       </c>
-      <c r="B211" s="7">
+      <c r="B211" s="6">
         <v>207.94900000000001</v>
       </c>
       <c r="C211">
@@ -9048,7 +9045,7 @@
       <c r="A212" s="5">
         <v>39234</v>
       </c>
-      <c r="B212" s="7">
+      <c r="B212" s="6">
         <v>208.352</v>
       </c>
       <c r="C212">
@@ -9064,7 +9061,7 @@
       <c r="A213" s="5">
         <v>39264</v>
       </c>
-      <c r="B213" s="7">
+      <c r="B213" s="6">
         <v>208.29900000000001</v>
       </c>
       <c r="C213">
@@ -9080,7 +9077,7 @@
       <c r="A214" s="5">
         <v>39295</v>
       </c>
-      <c r="B214" s="7">
+      <c r="B214" s="6">
         <v>207.917</v>
       </c>
       <c r="C214">
@@ -9096,7 +9093,7 @@
       <c r="A215" s="5">
         <v>39326</v>
       </c>
-      <c r="B215" s="7">
+      <c r="B215" s="6">
         <v>208.49</v>
       </c>
       <c r="C215">
@@ -9112,7 +9109,7 @@
       <c r="A216" s="5">
         <v>39356</v>
       </c>
-      <c r="B216" s="7">
+      <c r="B216" s="6">
         <v>208.93600000000001</v>
       </c>
       <c r="C216">
@@ -9128,7 +9125,7 @@
       <c r="A217" s="5">
         <v>39387</v>
       </c>
-      <c r="B217" s="7">
+      <c r="B217" s="6">
         <v>210.17699999999999</v>
       </c>
       <c r="C217">
@@ -9144,7 +9141,7 @@
       <c r="A218" s="5">
         <v>39417</v>
       </c>
-      <c r="B218" s="7">
+      <c r="B218" s="6">
         <v>210.036</v>
       </c>
       <c r="C218">
@@ -9160,7 +9157,7 @@
       <c r="A219" s="5">
         <v>39448</v>
       </c>
-      <c r="B219" s="7">
+      <c r="B219" s="6">
         <v>211.08</v>
       </c>
       <c r="C219">
@@ -9176,7 +9173,7 @@
       <c r="A220" s="5">
         <v>39479</v>
       </c>
-      <c r="B220" s="7">
+      <c r="B220" s="6">
         <v>211.69300000000001</v>
       </c>
       <c r="C220">
@@ -9192,7 +9189,7 @@
       <c r="A221" s="5">
         <v>39508</v>
       </c>
-      <c r="B221" s="7">
+      <c r="B221" s="6">
         <v>213.52799999999999</v>
       </c>
       <c r="C221">
@@ -9208,7 +9205,7 @@
       <c r="A222" s="5">
         <v>39539</v>
       </c>
-      <c r="B222" s="7">
+      <c r="B222" s="6">
         <v>214.82300000000001</v>
       </c>
       <c r="C222">
@@ -9224,7 +9221,7 @@
       <c r="A223" s="5">
         <v>39569</v>
       </c>
-      <c r="B223" s="7">
+      <c r="B223" s="6">
         <v>216.63200000000001</v>
       </c>
       <c r="C223">
@@ -9240,7 +9237,7 @@
       <c r="A224" s="5">
         <v>39600</v>
       </c>
-      <c r="B224" s="7">
+      <c r="B224" s="6">
         <v>218.815</v>
       </c>
       <c r="C224">
@@ -9256,7 +9253,7 @@
       <c r="A225" s="5">
         <v>39630</v>
       </c>
-      <c r="B225" s="7">
+      <c r="B225" s="6">
         <v>219.964</v>
       </c>
       <c r="C225">
@@ -9272,7 +9269,7 @@
       <c r="A226" s="5">
         <v>39661</v>
       </c>
-      <c r="B226" s="7">
+      <c r="B226" s="6">
         <v>219.08600000000001</v>
       </c>
       <c r="C226">
@@ -9288,7 +9285,7 @@
       <c r="A227" s="5">
         <v>39692</v>
       </c>
-      <c r="B227" s="7">
+      <c r="B227" s="6">
         <v>218.78299999999999</v>
       </c>
       <c r="C227">
@@ -9304,7 +9301,7 @@
       <c r="A228" s="5">
         <v>39722</v>
       </c>
-      <c r="B228" s="7">
+      <c r="B228" s="6">
         <v>216.57300000000001</v>
       </c>
       <c r="C228">
@@ -9320,7 +9317,7 @@
       <c r="A229" s="5">
         <v>39753</v>
       </c>
-      <c r="B229" s="7">
+      <c r="B229" s="6">
         <v>212.42500000000001</v>
       </c>
       <c r="C229">
@@ -9336,7 +9333,7 @@
       <c r="A230" s="5">
         <v>39783</v>
       </c>
-      <c r="B230" s="7">
+      <c r="B230" s="6">
         <v>210.22800000000001</v>
       </c>
       <c r="C230">
@@ -9352,7 +9349,7 @@
       <c r="A231" s="5">
         <v>39814</v>
       </c>
-      <c r="B231" s="7">
+      <c r="B231" s="6">
         <v>211.143</v>
       </c>
       <c r="C231">
@@ -9368,7 +9365,7 @@
       <c r="A232" s="5">
         <v>39845</v>
       </c>
-      <c r="B232" s="7">
+      <c r="B232" s="6">
         <v>212.19300000000001</v>
       </c>
       <c r="C232">
@@ -9384,7 +9381,7 @@
       <c r="A233" s="5">
         <v>39873</v>
       </c>
-      <c r="B233" s="7">
+      <c r="B233" s="6">
         <v>212.709</v>
       </c>
       <c r="C233">
@@ -9400,7 +9397,7 @@
       <c r="A234" s="5">
         <v>39904</v>
       </c>
-      <c r="B234" s="7">
+      <c r="B234" s="6">
         <v>213.24</v>
       </c>
       <c r="C234">
@@ -9416,7 +9413,7 @@
       <c r="A235" s="5">
         <v>39934</v>
       </c>
-      <c r="B235" s="7">
+      <c r="B235" s="6">
         <v>213.85599999999999</v>
       </c>
       <c r="C235">
@@ -9432,7 +9429,7 @@
       <c r="A236" s="5">
         <v>39965</v>
       </c>
-      <c r="B236" s="7">
+      <c r="B236" s="6">
         <v>215.69300000000001</v>
       </c>
       <c r="C236">
@@ -9448,7 +9445,7 @@
       <c r="A237" s="5">
         <v>39995</v>
       </c>
-      <c r="B237" s="7">
+      <c r="B237" s="6">
         <v>215.351</v>
       </c>
       <c r="C237">
@@ -9464,7 +9461,7 @@
       <c r="A238" s="5">
         <v>40026</v>
       </c>
-      <c r="B238" s="7">
+      <c r="B238" s="6">
         <v>215.834</v>
       </c>
       <c r="C238">
@@ -9480,7 +9477,7 @@
       <c r="A239" s="5">
         <v>40057</v>
       </c>
-      <c r="B239" s="7">
+      <c r="B239" s="6">
         <v>215.96899999999999</v>
       </c>
       <c r="C239">
@@ -9496,7 +9493,7 @@
       <c r="A240" s="5">
         <v>40087</v>
       </c>
-      <c r="B240" s="7">
+      <c r="B240" s="6">
         <v>216.17699999999999</v>
       </c>
       <c r="C240">
@@ -9512,7 +9509,7 @@
       <c r="A241" s="5">
         <v>40118</v>
       </c>
-      <c r="B241" s="7">
+      <c r="B241" s="6">
         <v>216.33</v>
       </c>
       <c r="C241">
@@ -9528,7 +9525,7 @@
       <c r="A242" s="5">
         <v>40148</v>
       </c>
-      <c r="B242" s="7">
+      <c r="B242" s="6">
         <v>215.94900000000001</v>
       </c>
       <c r="C242">
@@ -9544,7 +9541,7 @@
       <c r="A243" s="5">
         <v>40179</v>
       </c>
-      <c r="B243" s="7">
+      <c r="B243" s="6">
         <v>216.68700000000001</v>
       </c>
       <c r="C243">
@@ -9560,7 +9557,7 @@
       <c r="A244" s="5">
         <v>40210</v>
       </c>
-      <c r="B244" s="7">
+      <c r="B244" s="6">
         <v>216.74100000000001</v>
       </c>
       <c r="C244">
@@ -9576,7 +9573,7 @@
       <c r="A245" s="5">
         <v>40238</v>
       </c>
-      <c r="B245" s="7">
+      <c r="B245" s="6">
         <v>217.631</v>
       </c>
       <c r="C245">
@@ -9592,7 +9589,7 @@
       <c r="A246" s="5">
         <v>40269</v>
       </c>
-      <c r="B246" s="7">
+      <c r="B246" s="6">
         <v>218.00899999999999</v>
       </c>
       <c r="C246">
@@ -9608,7 +9605,7 @@
       <c r="A247" s="5">
         <v>40299</v>
       </c>
-      <c r="B247" s="7">
+      <c r="B247" s="6">
         <v>218.178</v>
       </c>
       <c r="C247">
@@ -9624,7 +9621,7 @@
       <c r="A248" s="5">
         <v>40330</v>
       </c>
-      <c r="B248" s="7">
+      <c r="B248" s="6">
         <v>217.965</v>
       </c>
       <c r="C248">
@@ -9640,7 +9637,7 @@
       <c r="A249" s="5">
         <v>40360</v>
       </c>
-      <c r="B249" s="7">
+      <c r="B249" s="6">
         <v>218.011</v>
       </c>
       <c r="C249">
@@ -9656,7 +9653,7 @@
       <c r="A250" s="5">
         <v>40391</v>
       </c>
-      <c r="B250" s="7">
+      <c r="B250" s="6">
         <v>218.31200000000001</v>
       </c>
       <c r="C250">
@@ -9672,7 +9669,7 @@
       <c r="A251" s="5">
         <v>40422</v>
       </c>
-      <c r="B251" s="7">
+      <c r="B251" s="6">
         <v>218.43899999999999</v>
       </c>
       <c r="C251">
@@ -9688,7 +9685,7 @@
       <c r="A252" s="5">
         <v>40452</v>
       </c>
-      <c r="B252" s="7">
+      <c r="B252" s="6">
         <v>218.71100000000001</v>
       </c>
       <c r="C252">
@@ -9704,7 +9701,7 @@
       <c r="A253" s="5">
         <v>40483</v>
       </c>
-      <c r="B253" s="7">
+      <c r="B253" s="6">
         <v>218.803</v>
       </c>
       <c r="C253">
@@ -9720,7 +9717,7 @@
       <c r="A254" s="5">
         <v>40513</v>
       </c>
-      <c r="B254" s="7">
+      <c r="B254" s="6">
         <v>219.179</v>
       </c>
       <c r="C254">
@@ -9736,7 +9733,7 @@
       <c r="A255" s="5">
         <v>40544</v>
       </c>
-      <c r="B255" s="7">
+      <c r="B255" s="6">
         <v>220.22300000000001</v>
       </c>
       <c r="C255">
@@ -9752,7 +9749,7 @@
       <c r="A256" s="5">
         <v>40575</v>
       </c>
-      <c r="B256" s="7">
+      <c r="B256" s="6">
         <v>221.309</v>
       </c>
       <c r="C256">
@@ -9768,7 +9765,7 @@
       <c r="A257" s="5">
         <v>40603</v>
       </c>
-      <c r="B257" s="7">
+      <c r="B257" s="6">
         <v>223.46700000000001</v>
       </c>
       <c r="C257">
@@ -9784,7 +9781,7 @@
       <c r="A258" s="5">
         <v>40634</v>
       </c>
-      <c r="B258" s="7">
+      <c r="B258" s="6">
         <v>224.90600000000001</v>
       </c>
       <c r="C258">
@@ -9800,7 +9797,7 @@
       <c r="A259" s="5">
         <v>40664</v>
       </c>
-      <c r="B259" s="7">
+      <c r="B259" s="6">
         <v>225.964</v>
       </c>
       <c r="C259">
@@ -9816,7 +9813,7 @@
       <c r="A260" s="5">
         <v>40695</v>
       </c>
-      <c r="B260" s="7">
+      <c r="B260" s="6">
         <v>225.72200000000001</v>
       </c>
       <c r="C260">
@@ -9832,7 +9829,7 @@
       <c r="A261" s="5">
         <v>40725</v>
       </c>
-      <c r="B261" s="7">
+      <c r="B261" s="6">
         <v>225.922</v>
       </c>
       <c r="C261">
@@ -9848,7 +9845,7 @@
       <c r="A262" s="5">
         <v>40756</v>
       </c>
-      <c r="B262" s="7">
+      <c r="B262" s="6">
         <v>226.54499999999999</v>
       </c>
       <c r="C262">
@@ -9864,7 +9861,7 @@
       <c r="A263" s="5">
         <v>40787</v>
       </c>
-      <c r="B263" s="7">
+      <c r="B263" s="6">
         <v>226.88900000000001</v>
       </c>
       <c r="C263">
@@ -9880,7 +9877,7 @@
       <c r="A264" s="5">
         <v>40817</v>
       </c>
-      <c r="B264" s="7">
+      <c r="B264" s="6">
         <v>226.42099999999999</v>
       </c>
       <c r="C264">
@@ -9896,7 +9893,7 @@
       <c r="A265" s="5">
         <v>40848</v>
       </c>
-      <c r="B265" s="7">
+      <c r="B265" s="6">
         <v>226.23</v>
       </c>
       <c r="C265">
@@ -9912,7 +9909,7 @@
       <c r="A266" s="5">
         <v>40878</v>
       </c>
-      <c r="B266" s="7">
+      <c r="B266" s="6">
         <v>225.672</v>
       </c>
       <c r="C266">
@@ -9928,7 +9925,7 @@
       <c r="A267" s="5">
         <v>40909</v>
       </c>
-      <c r="B267" s="7">
+      <c r="B267" s="6">
         <v>226.66499999999999</v>
       </c>
       <c r="C267">
@@ -9944,7 +9941,7 @@
       <c r="A268" s="5">
         <v>40940</v>
       </c>
-      <c r="B268" s="7">
+      <c r="B268" s="6">
         <v>227.66300000000001</v>
       </c>
       <c r="C268">
@@ -9960,7 +9957,7 @@
       <c r="A269" s="5">
         <v>40969</v>
       </c>
-      <c r="B269" s="7">
+      <c r="B269" s="6">
         <v>229.392</v>
       </c>
       <c r="C269">
@@ -9976,7 +9973,7 @@
       <c r="A270" s="5">
         <v>41000</v>
       </c>
-      <c r="B270" s="7">
+      <c r="B270" s="6">
         <v>230.08500000000001</v>
       </c>
       <c r="C270">
@@ -9992,7 +9989,7 @@
       <c r="A271" s="5">
         <v>41030</v>
       </c>
-      <c r="B271" s="7">
+      <c r="B271" s="6">
         <v>229.815</v>
       </c>
       <c r="C271">
@@ -10008,7 +10005,7 @@
       <c r="A272" s="5">
         <v>41061</v>
       </c>
-      <c r="B272" s="7">
+      <c r="B272" s="6">
         <v>229.47800000000001</v>
       </c>
       <c r="C272">
@@ -10024,7 +10021,7 @@
       <c r="A273" s="5">
         <v>41091</v>
       </c>
-      <c r="B273" s="7">
+      <c r="B273" s="6">
         <v>229.10400000000001</v>
       </c>
       <c r="C273">
@@ -10040,7 +10037,7 @@
       <c r="A274" s="5">
         <v>41122</v>
       </c>
-      <c r="B274" s="7">
+      <c r="B274" s="6">
         <v>230.37899999999999</v>
       </c>
       <c r="C274">
@@ -10056,7 +10053,7 @@
       <c r="A275" s="5">
         <v>41153</v>
       </c>
-      <c r="B275" s="7">
+      <c r="B275" s="6">
         <v>231.40700000000001</v>
       </c>
       <c r="C275">
@@ -10072,7 +10069,7 @@
       <c r="A276" s="5">
         <v>41183</v>
       </c>
-      <c r="B276" s="7">
+      <c r="B276" s="6">
         <v>231.31700000000001</v>
       </c>
       <c r="C276">
@@ -10088,7 +10085,7 @@
       <c r="A277" s="5">
         <v>41214</v>
       </c>
-      <c r="B277" s="7">
+      <c r="B277" s="6">
         <v>230.221</v>
       </c>
       <c r="C277">
@@ -10104,7 +10101,7 @@
       <c r="A278" s="5">
         <v>41244</v>
       </c>
-      <c r="B278" s="7">
+      <c r="B278" s="6">
         <v>229.601</v>
       </c>
       <c r="C278">
@@ -10120,7 +10117,7 @@
       <c r="A279" s="5">
         <v>41275</v>
       </c>
-      <c r="B279" s="7">
+      <c r="B279" s="6">
         <v>230.28</v>
       </c>
       <c r="C279">
@@ -10136,7 +10133,7 @@
       <c r="A280" s="5">
         <v>41306</v>
       </c>
-      <c r="B280" s="7">
+      <c r="B280" s="6">
         <v>232.166</v>
       </c>
       <c r="C280">
@@ -10152,7 +10149,7 @@
       <c r="A281" s="5">
         <v>41334</v>
       </c>
-      <c r="B281" s="7">
+      <c r="B281" s="6">
         <v>232.773</v>
       </c>
       <c r="C281">
@@ -10168,7 +10165,7 @@
       <c r="A282" s="5">
         <v>41365</v>
       </c>
-      <c r="B282" s="7">
+      <c r="B282" s="6">
         <v>232.53100000000001</v>
       </c>
       <c r="C282">
@@ -10184,7 +10181,7 @@
       <c r="A283" s="5">
         <v>41395</v>
       </c>
-      <c r="B283" s="7">
+      <c r="B283" s="6">
         <v>232.94499999999999</v>
       </c>
       <c r="C283">
@@ -10200,7 +10197,7 @@
       <c r="A284" s="5">
         <v>41426</v>
       </c>
-      <c r="B284" s="7">
+      <c r="B284" s="6">
         <v>233.50399999999999</v>
       </c>
       <c r="C284">
@@ -10216,7 +10213,7 @@
       <c r="A285" s="5">
         <v>41456</v>
       </c>
-      <c r="B285" s="7">
+      <c r="B285" s="6">
         <v>233.596</v>
       </c>
       <c r="C285">
@@ -10232,7 +10229,7 @@
       <c r="A286" s="5">
         <v>41487</v>
       </c>
-      <c r="B286" s="7">
+      <c r="B286" s="6">
         <v>233.87700000000001</v>
       </c>
       <c r="C286">
@@ -10248,7 +10245,7 @@
       <c r="A287" s="5">
         <v>41518</v>
       </c>
-      <c r="B287" s="7">
+      <c r="B287" s="6">
         <v>234.149</v>
       </c>
       <c r="C287">
@@ -10264,7 +10261,7 @@
       <c r="A288" s="5">
         <v>41548</v>
       </c>
-      <c r="B288" s="7">
+      <c r="B288" s="6">
         <v>233.54599999999999</v>
       </c>
       <c r="C288">
@@ -10280,7 +10277,7 @@
       <c r="A289" s="5">
         <v>41579</v>
       </c>
-      <c r="B289" s="7">
+      <c r="B289" s="6">
         <v>233.06899999999999</v>
       </c>
       <c r="C289">
@@ -10296,7 +10293,7 @@
       <c r="A290" s="5">
         <v>41609</v>
       </c>
-      <c r="B290" s="7">
+      <c r="B290" s="6">
         <v>233.04900000000001</v>
       </c>
       <c r="C290">
@@ -10312,7 +10309,7 @@
       <c r="A291" s="5">
         <v>41640</v>
       </c>
-      <c r="B291" s="7">
+      <c r="B291" s="6">
         <v>233.916</v>
       </c>
       <c r="C291">
@@ -10328,7 +10325,7 @@
       <c r="A292" s="5">
         <v>41671</v>
       </c>
-      <c r="B292" s="7">
+      <c r="B292" s="6">
         <v>234.78100000000001</v>
       </c>
       <c r="C292">
@@ -10344,7 +10341,7 @@
       <c r="A293" s="5">
         <v>41699</v>
       </c>
-      <c r="B293" s="7">
+      <c r="B293" s="6">
         <v>236.29300000000001</v>
       </c>
       <c r="C293">
@@ -10360,7 +10357,7 @@
       <c r="A294" s="5">
         <v>41730</v>
       </c>
-      <c r="B294" s="7">
+      <c r="B294" s="6">
         <v>237.072</v>
       </c>
       <c r="C294">
@@ -10376,7 +10373,7 @@
       <c r="A295" s="5">
         <v>41760</v>
       </c>
-      <c r="B295" s="7">
+      <c r="B295" s="6">
         <v>237.9</v>
       </c>
       <c r="C295">
@@ -10392,7 +10389,7 @@
       <c r="A296" s="5">
         <v>41791</v>
       </c>
-      <c r="B296" s="7">
+      <c r="B296" s="6">
         <v>238.34299999999999</v>
       </c>
       <c r="C296">
@@ -10408,7 +10405,7 @@
       <c r="A297" s="5">
         <v>41821</v>
       </c>
-      <c r="B297" s="7">
+      <c r="B297" s="6">
         <v>238.25</v>
       </c>
       <c r="C297">
@@ -10424,7 +10421,7 @@
       <c r="A298" s="5">
         <v>41852</v>
       </c>
-      <c r="B298" s="7">
+      <c r="B298" s="6">
         <v>237.852</v>
       </c>
       <c r="C298">
@@ -10440,7 +10437,7 @@
       <c r="A299" s="5">
         <v>41883</v>
       </c>
-      <c r="B299" s="7">
+      <c r="B299" s="6">
         <v>238.03100000000001</v>
       </c>
       <c r="C299">
@@ -10456,7 +10453,7 @@
       <c r="A300" s="5">
         <v>41913</v>
       </c>
-      <c r="B300" s="7">
+      <c r="B300" s="6">
         <v>237.43299999999999</v>
       </c>
       <c r="C300">
@@ -10472,7 +10469,7 @@
       <c r="A301" s="5">
         <v>41944</v>
       </c>
-      <c r="B301" s="7">
+      <c r="B301" s="6">
         <v>236.15100000000001</v>
       </c>
       <c r="C301">
@@ -10488,7 +10485,7 @@
       <c r="A302" s="5">
         <v>41974</v>
       </c>
-      <c r="B302" s="7">
+      <c r="B302" s="6">
         <v>234.81200000000001</v>
       </c>
       <c r="C302">
@@ -10504,7 +10501,7 @@
       <c r="A303" s="5">
         <v>42005</v>
       </c>
-      <c r="B303" s="7">
+      <c r="B303" s="6">
         <v>233.70699999999999</v>
       </c>
       <c r="C303">
@@ -10520,7 +10517,7 @@
       <c r="A304" s="5">
         <v>42036</v>
       </c>
-      <c r="B304" s="7">
+      <c r="B304" s="6">
         <v>234.72200000000001</v>
       </c>
       <c r="C304">
@@ -10536,7 +10533,7 @@
       <c r="A305" s="5">
         <v>42064</v>
       </c>
-      <c r="B305" s="7">
+      <c r="B305" s="6">
         <v>236.119</v>
       </c>
       <c r="C305">
@@ -10552,7 +10549,7 @@
       <c r="A306" s="5">
         <v>42095</v>
       </c>
-      <c r="B306" s="7">
+      <c r="B306" s="6">
         <v>236.59899999999999</v>
       </c>
       <c r="C306">
@@ -10568,7 +10565,7 @@
       <c r="A307" s="5">
         <v>42125</v>
       </c>
-      <c r="B307" s="7">
+      <c r="B307" s="6">
         <v>237.80500000000001</v>
       </c>
       <c r="C307">
@@ -10584,7 +10581,7 @@
       <c r="A308" s="5">
         <v>42156</v>
       </c>
-      <c r="B308" s="7">
+      <c r="B308" s="6">
         <v>238.63800000000001</v>
       </c>
       <c r="C308">
@@ -10600,7 +10597,7 @@
       <c r="A309" s="5">
         <v>42186</v>
       </c>
-      <c r="B309" s="7">
+      <c r="B309" s="6">
         <v>238.654</v>
       </c>
       <c r="C309">
@@ -10616,7 +10613,7 @@
       <c r="A310" s="5">
         <v>42217</v>
       </c>
-      <c r="B310" s="7">
+      <c r="B310" s="6">
         <v>238.316</v>
       </c>
       <c r="C310">
@@ -10632,7 +10629,7 @@
       <c r="A311" s="5">
         <v>42248</v>
       </c>
-      <c r="B311" s="7">
+      <c r="B311" s="6">
         <v>237.94499999999999</v>
       </c>
       <c r="C311">
@@ -10648,7 +10645,7 @@
       <c r="A312" s="5">
         <v>42278</v>
       </c>
-      <c r="B312" s="7">
+      <c r="B312" s="6">
         <v>237.83799999999999</v>
       </c>
       <c r="C312">
@@ -10664,7 +10661,7 @@
       <c r="A313" s="5">
         <v>42309</v>
       </c>
-      <c r="B313" s="7">
+      <c r="B313" s="6">
         <v>237.33600000000001</v>
       </c>
       <c r="C313">
@@ -10680,7 +10677,7 @@
       <c r="A314" s="5">
         <v>42339</v>
       </c>
-      <c r="B314" s="7">
+      <c r="B314" s="6">
         <v>236.52500000000001</v>
       </c>
       <c r="C314">
@@ -10696,7 +10693,7 @@
       <c r="A315" s="5">
         <v>42370</v>
       </c>
-      <c r="B315" s="7">
+      <c r="B315" s="6">
         <v>236.916</v>
       </c>
       <c r="C315">
@@ -10712,7 +10709,7 @@
       <c r="A316" s="5">
         <v>42401</v>
       </c>
-      <c r="B316" s="7">
+      <c r="B316" s="6">
         <v>237.11099999999999</v>
       </c>
       <c r="C316">
@@ -10728,7 +10725,7 @@
       <c r="A317" s="5">
         <v>42430</v>
       </c>
-      <c r="B317" s="7">
+      <c r="B317" s="6">
         <v>238.13200000000001</v>
       </c>
       <c r="C317">
@@ -10744,7 +10741,7 @@
       <c r="A318" s="5">
         <v>42461</v>
       </c>
-      <c r="B318" s="7">
+      <c r="B318" s="6">
         <v>239.261</v>
       </c>
       <c r="C318">
@@ -10760,7 +10757,7 @@
       <c r="A319" s="5">
         <v>42491</v>
       </c>
-      <c r="B319" s="7">
+      <c r="B319" s="6">
         <v>240.22900000000001</v>
       </c>
       <c r="C319">
@@ -10776,7 +10773,7 @@
       <c r="A320" s="5">
         <v>42522</v>
       </c>
-      <c r="B320" s="7">
+      <c r="B320" s="6">
         <v>241.018</v>
       </c>
       <c r="C320">
@@ -10792,7 +10789,7 @@
       <c r="A321" s="5">
         <v>42552</v>
       </c>
-      <c r="B321" s="7">
+      <c r="B321" s="6">
         <v>240.62799999999999</v>
       </c>
       <c r="C321">
@@ -10808,7 +10805,7 @@
       <c r="A322" s="5">
         <v>42583</v>
       </c>
-      <c r="B322" s="7">
+      <c r="B322" s="6">
         <v>240.84899999999999</v>
       </c>
       <c r="C322">
@@ -10824,7 +10821,7 @@
       <c r="A323" s="5">
         <v>42614</v>
       </c>
-      <c r="B323" s="7">
+      <c r="B323" s="6">
         <v>241.428</v>
       </c>
       <c r="C323">
@@ -10840,7 +10837,7 @@
       <c r="A324" s="5">
         <v>42644</v>
       </c>
-      <c r="B324" s="7">
+      <c r="B324" s="6">
         <v>241.72900000000001</v>
       </c>
       <c r="C324">
@@ -10856,7 +10853,7 @@
       <c r="A325" s="5">
         <v>42675</v>
       </c>
-      <c r="B325" s="7">
+      <c r="B325" s="6">
         <v>241.35300000000001</v>
       </c>
       <c r="C325">
@@ -10872,7 +10869,7 @@
       <c r="A326" s="5">
         <v>42705</v>
       </c>
-      <c r="B326" s="7">
+      <c r="B326" s="6">
         <v>241.43199999999999</v>
       </c>
       <c r="C326">
@@ -10888,7 +10885,7 @@
       <c r="A327" s="5">
         <v>42736</v>
       </c>
-      <c r="B327" s="7">
+      <c r="B327" s="6">
         <v>242.839</v>
       </c>
       <c r="C327">
@@ -10904,7 +10901,7 @@
       <c r="A328" s="5">
         <v>42767</v>
       </c>
-      <c r="B328" s="7">
+      <c r="B328" s="6">
         <v>243.60300000000001</v>
       </c>
       <c r="C328">
@@ -10920,7 +10917,7 @@
       <c r="A329" s="5">
         <v>42795</v>
       </c>
-      <c r="B329" s="7">
+      <c r="B329" s="6">
         <v>243.80099999999999</v>
       </c>
       <c r="C329">
@@ -10936,7 +10933,7 @@
       <c r="A330" s="5">
         <v>42826</v>
       </c>
-      <c r="B330" s="7">
+      <c r="B330" s="6">
         <v>244.524</v>
       </c>
       <c r="C330">
@@ -10952,7 +10949,7 @@
       <c r="A331" s="5">
         <v>42856</v>
       </c>
-      <c r="B331" s="7">
+      <c r="B331" s="6">
         <v>244.733</v>
       </c>
       <c r="C331">
@@ -10968,7 +10965,7 @@
       <c r="A332" s="5">
         <v>42887</v>
       </c>
-      <c r="B332" s="7">
+      <c r="B332" s="6">
         <v>244.95500000000001</v>
       </c>
       <c r="C332">
@@ -10984,7 +10981,7 @@
       <c r="A333" s="5">
         <v>42917</v>
       </c>
-      <c r="B333" s="7">
+      <c r="B333" s="6">
         <v>244.786</v>
       </c>
       <c r="C333">
@@ -11000,7 +10997,7 @@
       <c r="A334" s="5">
         <v>42948</v>
       </c>
-      <c r="B334" s="7">
+      <c r="B334" s="6">
         <v>245.51900000000001</v>
       </c>
       <c r="C334">
@@ -11016,7 +11013,7 @@
       <c r="A335" s="5">
         <v>42979</v>
       </c>
-      <c r="B335" s="7">
+      <c r="B335" s="6">
         <v>246.81899999999999</v>
       </c>
       <c r="C335">
@@ -11032,7 +11029,7 @@
       <c r="A336" s="5">
         <v>43009</v>
       </c>
-      <c r="B336" s="7">
+      <c r="B336" s="6">
         <v>246.66300000000001</v>
       </c>
       <c r="C336">
@@ -11048,7 +11045,7 @@
       <c r="A337" s="5">
         <v>43040</v>
       </c>
-      <c r="B337" s="7">
+      <c r="B337" s="6">
         <v>246.66900000000001</v>
       </c>
       <c r="C337">
@@ -11064,7 +11061,7 @@
       <c r="A338" s="5">
         <v>43070</v>
       </c>
-      <c r="B338" s="7">
+      <c r="B338" s="6">
         <v>246.524</v>
       </c>
       <c r="C338">
@@ -11080,7 +11077,7 @@
       <c r="A339" s="5">
         <v>43101</v>
       </c>
-      <c r="B339" s="7">
+      <c r="B339" s="6">
         <v>247.86699999999999</v>
       </c>
       <c r="C339">
@@ -11096,7 +11093,7 @@
       <c r="A340" s="5">
         <v>43132</v>
       </c>
-      <c r="B340" s="7">
+      <c r="B340" s="6">
         <v>248.99100000000001</v>
       </c>
       <c r="C340">
@@ -11112,7 +11109,7 @@
       <c r="A341" s="5">
         <v>43160</v>
       </c>
-      <c r="B341" s="7">
+      <c r="B341" s="6">
         <v>249.554</v>
       </c>
       <c r="C341">
@@ -11128,7 +11125,7 @@
       <c r="A342" s="5">
         <v>43191</v>
       </c>
-      <c r="B342" s="7">
+      <c r="B342" s="6">
         <v>250.54599999999999</v>
       </c>
       <c r="C342">
@@ -11144,7 +11141,7 @@
       <c r="A343" s="5">
         <v>43221</v>
       </c>
-      <c r="B343" s="7">
+      <c r="B343" s="6">
         <v>251.58799999999999</v>
       </c>
       <c r="C343">
@@ -11160,7 +11157,7 @@
       <c r="A344" s="5">
         <v>43252</v>
       </c>
-      <c r="B344" s="7">
+      <c r="B344" s="6">
         <v>251.989</v>
       </c>
       <c r="C344">
@@ -11176,7 +11173,7 @@
       <c r="A345" s="5">
         <v>43282</v>
       </c>
-      <c r="B345" s="7">
+      <c r="B345" s="6">
         <v>252.006</v>
       </c>
       <c r="C345">
@@ -11192,7 +11189,7 @@
       <c r="A346" s="5">
         <v>43313</v>
       </c>
-      <c r="B346" s="7">
+      <c r="B346" s="6">
         <v>252.14599999999999</v>
       </c>
       <c r="C346">
@@ -11208,7 +11205,7 @@
       <c r="A347" s="5">
         <v>43344</v>
       </c>
-      <c r="B347" s="7">
+      <c r="B347" s="6">
         <v>252.43899999999999</v>
       </c>
       <c r="C347">
@@ -11224,7 +11221,7 @@
       <c r="A348" s="5">
         <v>43374</v>
       </c>
-      <c r="B348" s="7">
+      <c r="B348" s="6">
         <v>252.88499999999999</v>
       </c>
       <c r="C348">
@@ -11240,7 +11237,7 @@
       <c r="A349" s="5">
         <v>43405</v>
       </c>
-      <c r="B349" s="7">
+      <c r="B349" s="6">
         <v>252.03800000000001</v>
       </c>
       <c r="C349">
@@ -11256,7 +11253,7 @@
       <c r="A350" s="5">
         <v>43435</v>
       </c>
-      <c r="B350" s="7">
+      <c r="B350" s="6">
         <v>251.233</v>
       </c>
       <c r="C350">
@@ -11272,7 +11269,7 @@
       <c r="A351" s="5">
         <v>43466</v>
       </c>
-      <c r="B351" s="7">
+      <c r="B351" s="6">
         <v>251.71199999999999</v>
       </c>
       <c r="C351">
@@ -11288,7 +11285,7 @@
       <c r="A352" s="5">
         <v>43497</v>
       </c>
-      <c r="B352" s="7">
+      <c r="B352" s="6">
         <v>252.77600000000001</v>
       </c>
       <c r="C352">
@@ -11304,7 +11301,7 @@
       <c r="A353" s="5">
         <v>43525</v>
       </c>
-      <c r="B353" s="7">
+      <c r="B353" s="6">
         <v>254.202</v>
       </c>
       <c r="C353">
@@ -11320,7 +11317,7 @@
       <c r="A354" s="5">
         <v>43556</v>
       </c>
-      <c r="B354" s="7">
+      <c r="B354" s="6">
         <v>255.548</v>
       </c>
       <c r="C354">
@@ -11336,7 +11333,7 @@
       <c r="A355" s="5">
         <v>43586</v>
       </c>
-      <c r="B355" s="7">
+      <c r="B355" s="6">
         <v>256.09199999999998</v>
       </c>
       <c r="C355">
@@ -11352,7 +11349,7 @@
       <c r="A356" s="5">
         <v>43617</v>
       </c>
-      <c r="B356" s="7">
+      <c r="B356" s="6">
         <v>256.14299999999997</v>
       </c>
       <c r="C356">
@@ -11368,7 +11365,7 @@
       <c r="A357" s="5">
         <v>43647</v>
       </c>
-      <c r="B357" s="7">
+      <c r="B357" s="6">
         <v>256.57100000000003</v>
       </c>
       <c r="C357">
@@ -11384,7 +11381,7 @@
       <c r="A358" s="5">
         <v>43678</v>
       </c>
-      <c r="B358" s="7">
+      <c r="B358" s="6">
         <v>256.55799999999999</v>
       </c>
       <c r="C358">
@@ -11400,7 +11397,7 @@
       <c r="A359" s="5">
         <v>43709</v>
       </c>
-      <c r="B359" s="7">
+      <c r="B359" s="6">
         <v>256.75900000000001</v>
       </c>
       <c r="C359">
@@ -11416,7 +11413,7 @@
       <c r="A360" s="5">
         <v>43739</v>
       </c>
-      <c r="B360" s="7">
+      <c r="B360" s="6">
         <v>257.346</v>
       </c>
       <c r="C360">
@@ -11432,7 +11429,7 @@
       <c r="A361" s="5">
         <v>43770</v>
       </c>
-      <c r="B361" s="7">
+      <c r="B361" s="6">
         <v>257.20800000000003</v>
       </c>
       <c r="C361">
@@ -11448,7 +11445,7 @@
       <c r="A362" s="5">
         <v>43800</v>
       </c>
-      <c r="B362" s="7">
+      <c r="B362" s="6">
         <v>256.97399999999999</v>
       </c>
       <c r="C362">
@@ -11464,7 +11461,7 @@
       <c r="A363" s="5">
         <v>43831</v>
       </c>
-      <c r="B363" s="7">
+      <c r="B363" s="6">
         <v>257.971</v>
       </c>
       <c r="C363">
@@ -11480,7 +11477,7 @@
       <c r="A364" s="5">
         <v>43862</v>
       </c>
-      <c r="B364" s="7">
+      <c r="B364" s="6">
         <v>258.678</v>
       </c>
       <c r="C364">
@@ -11496,7 +11493,7 @@
       <c r="A365" s="5">
         <v>43891</v>
       </c>
-      <c r="B365" s="7">
+      <c r="B365" s="6">
         <v>258.11500000000001</v>
       </c>
       <c r="C365">
@@ -11512,7 +11509,7 @@
       <c r="A366" s="5">
         <v>43922</v>
       </c>
-      <c r="B366" s="7">
+      <c r="B366" s="6">
         <v>256.38900000000001</v>
       </c>
       <c r="C366">
@@ -11528,7 +11525,7 @@
       <c r="A367" s="5">
         <v>43952</v>
       </c>
-      <c r="B367" s="7">
+      <c r="B367" s="6">
         <v>256.39400000000001</v>
       </c>
       <c r="C367">
@@ -11544,7 +11541,7 @@
       <c r="A368" s="5">
         <v>43983</v>
       </c>
-      <c r="B368" s="7">
+      <c r="B368" s="6">
         <v>257.79700000000003</v>
       </c>
       <c r="C368">
@@ -11560,7 +11557,7 @@
       <c r="A369" s="5">
         <v>44013</v>
       </c>
-      <c r="B369" s="7">
+      <c r="B369" s="6">
         <v>259.101</v>
       </c>
       <c r="C369">
@@ -11576,7 +11573,7 @@
       <c r="A370" s="5">
         <v>44044</v>
       </c>
-      <c r="B370" s="7">
+      <c r="B370" s="6">
         <v>259.91800000000001</v>
       </c>
       <c r="C370">
@@ -11592,7 +11589,7 @@
       <c r="A371" s="5">
         <v>44075</v>
       </c>
-      <c r="B371" s="7">
+      <c r="B371" s="6">
         <v>260.27999999999997</v>
       </c>
       <c r="C371">
@@ -11608,7 +11605,7 @@
       <c r="A372" s="5">
         <v>44105</v>
       </c>
-      <c r="B372" s="7">
+      <c r="B372" s="6">
         <v>260.38799999999998</v>
       </c>
       <c r="C372">
@@ -11624,7 +11621,7 @@
       <c r="A373" s="5">
         <v>44136</v>
       </c>
-      <c r="B373" s="7">
+      <c r="B373" s="6">
         <v>260.22899999999998</v>
       </c>
       <c r="C373">
@@ -11640,7 +11637,7 @@
       <c r="A374" s="5">
         <v>44166</v>
       </c>
-      <c r="B374" s="7">
+      <c r="B374" s="6">
         <v>260.47399999999999</v>
       </c>
       <c r="C374">
@@ -11656,7 +11653,7 @@
       <c r="A375" s="5">
         <v>44197</v>
       </c>
-      <c r="B375" s="7">
+      <c r="B375" s="6">
         <v>261.58199999999999</v>
       </c>
       <c r="C375">
@@ -11672,7 +11669,7 @@
       <c r="A376" s="5">
         <v>44228</v>
       </c>
-      <c r="B376" s="7">
+      <c r="B376" s="6">
         <v>263.01400000000001</v>
       </c>
       <c r="C376">
@@ -11688,7 +11685,7 @@
       <c r="A377" s="5">
         <v>44256</v>
       </c>
-      <c r="B377" s="7">
+      <c r="B377" s="6">
         <v>264.87700000000001</v>
       </c>
       <c r="C377">
@@ -11704,7 +11701,7 @@
       <c r="A378" s="5">
         <v>44287</v>
       </c>
-      <c r="B378" s="7">
+      <c r="B378" s="6">
         <v>267.05399999999997</v>
       </c>
       <c r="C378">
@@ -11720,7 +11717,7 @@
       <c r="A379" s="5">
         <v>44317</v>
       </c>
-      <c r="B379" s="7">
+      <c r="B379" s="6">
         <v>269.19499999999999</v>
       </c>
       <c r="C379">
@@ -11736,7 +11733,7 @@
       <c r="A380" s="5">
         <v>44348</v>
       </c>
-      <c r="B380" s="7">
+      <c r="B380" s="6">
         <v>271.69600000000003</v>
       </c>
       <c r="C380">
@@ -11752,7 +11749,7 @@
       <c r="A381" s="5">
         <v>44378</v>
       </c>
-      <c r="B381" s="7">
+      <c r="B381" s="6">
         <v>273.00299999999999</v>
       </c>
       <c r="C381">
@@ -11768,7 +11765,7 @@
       <c r="A382" s="5">
         <v>44409</v>
       </c>
-      <c r="B382" s="7">
+      <c r="B382" s="6">
         <v>273.56700000000001</v>
       </c>
       <c r="C382">
@@ -11784,7 +11781,7 @@
       <c r="A383" s="5">
         <v>44440</v>
       </c>
-      <c r="B383" s="7">
+      <c r="B383" s="6">
         <v>274.31</v>
       </c>
       <c r="C383">
@@ -11800,7 +11797,7 @@
       <c r="A384" s="5">
         <v>44470</v>
       </c>
-      <c r="B384" s="7">
+      <c r="B384" s="6">
         <v>276.589</v>
       </c>
       <c r="C384">
@@ -11816,7 +11813,7 @@
       <c r="A385" s="5">
         <v>44501</v>
       </c>
-      <c r="B385" s="7">
+      <c r="B385" s="6">
         <v>277.94799999999998</v>
       </c>
       <c r="C385">
@@ -11832,7 +11829,7 @@
       <c r="A386" s="5">
         <v>44531</v>
       </c>
-      <c r="B386" s="7">
+      <c r="B386" s="6">
         <v>278.80200000000002</v>
       </c>
       <c r="C386">
@@ -11848,7 +11845,7 @@
       <c r="A387" s="5">
         <v>44562</v>
       </c>
-      <c r="B387" s="7">
+      <c r="B387" s="6">
         <v>281.14800000000002</v>
       </c>
       <c r="C387">
@@ -11864,7 +11861,7 @@
       <c r="A388" s="5">
         <v>44593</v>
       </c>
-      <c r="B388" s="7">
+      <c r="B388" s="6">
         <v>283.71600000000001</v>
       </c>
       <c r="C388">
@@ -11880,7 +11877,7 @@
       <c r="A389" s="5">
         <v>44621</v>
       </c>
-      <c r="B389" s="7">
+      <c r="B389" s="6">
         <v>287.50400000000002</v>
       </c>
       <c r="C389">
@@ -11896,7 +11893,7 @@
       <c r="A390" s="5">
         <v>44652</v>
       </c>
-      <c r="B390" s="7">
+      <c r="B390" s="6">
         <v>289.10899999999998</v>
       </c>
       <c r="C390">
@@ -11912,7 +11909,7 @@
       <c r="A391" s="5">
         <v>44682</v>
       </c>
-      <c r="B391" s="7">
+      <c r="B391" s="6">
         <v>292.29599999999999</v>
       </c>
       <c r="C391">
@@ -11928,7 +11925,7 @@
       <c r="A392" s="5">
         <v>44713</v>
       </c>
-      <c r="B392" s="7">
+      <c r="B392" s="6">
         <v>296.31099999999998</v>
       </c>
       <c r="C392">
@@ -11944,7 +11941,7 @@
       <c r="A393" s="5">
         <v>44743</v>
       </c>
-      <c r="B393" s="7">
+      <c r="B393" s="6">
         <v>296.27600000000001</v>
       </c>
       <c r="C393">
@@ -11960,7 +11957,7 @@
       <c r="A394" s="5">
         <v>44774</v>
       </c>
-      <c r="B394" s="7">
+      <c r="B394" s="6">
         <v>296.17099999999999</v>
       </c>
       <c r="C394">
@@ -11976,7 +11973,7 @@
       <c r="A395" s="5">
         <v>44805</v>
       </c>
-      <c r="B395" s="7">
+      <c r="B395" s="6">
         <v>296.80799999999999</v>
       </c>
       <c r="C395">
@@ -11992,7 +11989,7 @@
       <c r="A396" s="5">
         <v>44835</v>
       </c>
-      <c r="B396" s="7">
+      <c r="B396" s="6">
         <v>298.012</v>
       </c>
       <c r="C396">
@@ -12008,7 +12005,7 @@
       <c r="A397" s="5">
         <v>44866</v>
       </c>
-      <c r="B397" s="7">
+      <c r="B397" s="6">
         <v>297.71100000000001</v>
       </c>
       <c r="C397">
@@ -12024,7 +12021,7 @@
       <c r="A398" s="5">
         <v>44896</v>
       </c>
-      <c r="B398" s="7">
+      <c r="B398" s="6">
         <v>296.79700000000003</v>
       </c>
       <c r="C398">
@@ -12040,7 +12037,7 @@
       <c r="A399" s="5">
         <v>44927</v>
       </c>
-      <c r="B399" s="7">
+      <c r="B399" s="6">
         <v>299.17</v>
       </c>
       <c r="C399">
@@ -12056,7 +12053,7 @@
       <c r="A400" s="5">
         <v>44958</v>
       </c>
-      <c r="B400" s="7">
+      <c r="B400" s="6">
         <v>300.83999999999997</v>
       </c>
       <c r="C400">
@@ -12072,7 +12069,7 @@
       <c r="A401" s="5">
         <v>44986</v>
       </c>
-      <c r="B401" s="7">
+      <c r="B401" s="6">
         <v>301.83600000000001</v>
       </c>
       <c r="C401">
@@ -12088,7 +12085,7 @@
       <c r="A402" s="5">
         <v>45017</v>
       </c>
-      <c r="B402" s="7">
+      <c r="B402" s="6">
         <v>303.363</v>
       </c>
       <c r="C402">
@@ -12104,7 +12101,7 @@
       <c r="A403" s="5">
         <v>45047</v>
       </c>
-      <c r="B403" s="7">
+      <c r="B403" s="6">
         <v>304.12700000000001</v>
       </c>
       <c r="C403">

</xml_diff>

<commit_message>
added LSTM and GRU
</commit_message>
<xml_diff>
--- a/Data/EconomicData/MonthlyCPI-BLS.xlsx
+++ b/Data/EconomicData/MonthlyCPI-BLS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\OneDrive\Documents\CodingProjectsStuff\2023SummerResearch-Inflation\COVID-Inflation\Data\EconomicData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/47480c2cf74a22f9/Documents/CodingProjectsStuff/2023SummerResearch-Inflation/COVID-Inflation/Data/EconomicData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F41AD52-2C2E-4142-9D14-0C2FF6E0E404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="13_ncr:1_{1F41AD52-2C2E-4142-9D14-0C2FF6E0E404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20000ABE-FFC1-4533-AF2B-CC4B608314D8}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BLS Data Series" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Value</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>MoM-Annualized-Inflation</t>
+  </si>
+  <si>
+    <t>08-09 recession</t>
   </si>
 </sst>
 </file>
@@ -2176,6 +2179,35 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Month over Month Change</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> in CPI Inflation (Annualized)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2226,6 +2258,146 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="226"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.0185195493861946E-2"/>
+                  <c:y val="-2.048675988411269E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>11/2008:</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t> </a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>Inflation shock</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t> from the 2008-09 recession</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-E454-47FA-8DC6-96ABAD653B82}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="363"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.1268869030902611"/>
+                  <c:y val="3.1234127946152775E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>4/2020: Inflation shock from COVID-19</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-E454-47FA-8DC6-96ABAD653B82}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="25000"/>
+                    <a:lumOff val="75000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="wedgeRectCallout">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>'BLS Data Series'!$A$3:$A$403</c:f>
@@ -4694,7 +4866,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="b" anchorCtr="0"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -4718,6 +4890,8 @@
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
+        <c:majorUnit val="16"/>
+        <c:majorTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
         <c:axId val="1503606976"/>
@@ -4740,6 +4914,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>% Change in CPI Inflation (Annualized)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -5972,16 +6201,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>741044</xdr:colOff>
-      <xdr:row>367</xdr:row>
-      <xdr:rowOff>59053</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>765004</xdr:colOff>
+      <xdr:row>344</xdr:row>
+      <xdr:rowOff>88233</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>314324</xdr:colOff>
-      <xdr:row>403</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>368</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6004,15 +6233,159 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>347</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>449179</xdr:colOff>
+      <xdr:row>367</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0805349D-49E9-0A3A-9198-00CA062F8971}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10114547" y="64032063"/>
+          <a:ext cx="449179" cy="3689684"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+            <a:alpha val="48000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>346</xdr:row>
+      <xdr:rowOff>184483</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>367</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectangle 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E8CC1FE-3648-4C10-BD6E-1094203CC3C6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12857747" y="64032062"/>
+          <a:ext cx="914400" cy="3689685"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+            <a:alpha val="48000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -6050,7 +6423,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -6156,7 +6529,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6298,7 +6671,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -6306,11 +6679,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D403"/>
+  <dimension ref="A1:H403"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A361" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" activeCellId="1" sqref="A3:A403 D3:D403"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A343" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W357" sqref="W357"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6319,6 +6692,7 @@
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" customWidth="1"/>
     <col min="4" max="4" width="19.5546875" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -11687,7 +12061,7 @@
         <v>-0.75845052447328998</v>
       </c>
     </row>
-    <row r="337" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A337" s="5">
         <v>43040</v>
       </c>
@@ -11703,7 +12077,7 @@
         <v>2.9189623088992967E-2</v>
       </c>
     </row>
-    <row r="338" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A338" s="5">
         <v>43070</v>
       </c>
@@ -11719,7 +12093,7 @@
         <v>-0.70539873271474041</v>
       </c>
     </row>
-    <row r="339" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A339" s="5">
         <v>43101</v>
       </c>
@@ -11735,7 +12109,7 @@
         <v>6.5372945433304146</v>
       </c>
     </row>
-    <row r="340" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A340" s="5">
         <v>43132</v>
       </c>
@@ -11751,7 +12125,7 @@
         <v>5.4416279698387786</v>
       </c>
     </row>
-    <row r="341" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A341" s="5">
         <v>43160</v>
       </c>
@@ -11767,7 +12141,7 @@
         <v>2.7133510849789175</v>
       </c>
     </row>
-    <row r="342" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A342" s="5">
         <v>43191</v>
       </c>
@@ -11783,7 +12157,7 @@
         <v>4.7701098760187701</v>
       </c>
     </row>
-    <row r="343" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A343" s="5">
         <v>43221</v>
       </c>
@@ -11799,7 +12173,7 @@
         <v>4.9907003105218282</v>
       </c>
     </row>
-    <row r="344" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A344" s="5">
         <v>43252</v>
       </c>
@@ -11815,7 +12189,7 @@
         <v>1.9126508418526025</v>
       </c>
     </row>
-    <row r="345" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A345" s="5">
         <v>43282</v>
       </c>
@@ -11830,8 +12204,11 @@
         <f t="shared" si="11"/>
         <v>8.0955914742290691E-2</v>
       </c>
-    </row>
-    <row r="346" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G345" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="346" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A346" s="5">
         <v>43313</v>
       </c>
@@ -11846,8 +12223,15 @@
         <f t="shared" si="11"/>
         <v>0.66665079402864869</v>
       </c>
-    </row>
-    <row r="347" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G346" s="5">
+        <v>39417</v>
+      </c>
+      <c r="H346">
+        <f t="shared" ref="H346:H364" si="12">$C346*12</f>
+        <v>0.66665079402864869</v>
+      </c>
+    </row>
+    <row r="347" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A347" s="5">
         <v>43344</v>
       </c>
@@ -11862,8 +12246,15 @@
         <f t="shared" si="11"/>
         <v>1.394430211068221</v>
       </c>
-    </row>
-    <row r="348" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G347" s="5">
+        <v>39448</v>
+      </c>
+      <c r="H347">
+        <f t="shared" si="12"/>
+        <v>1.394430211068221</v>
+      </c>
+    </row>
+    <row r="348" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A348" s="5">
         <v>43374</v>
       </c>
@@ -11878,8 +12269,15 @@
         <f t="shared" si="11"/>
         <v>2.1201161468711156</v>
       </c>
-    </row>
-    <row r="349" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G348" s="5">
+        <v>39479</v>
+      </c>
+      <c r="H348">
+        <f t="shared" si="12"/>
+        <v>2.1201161468711156</v>
+      </c>
+    </row>
+    <row r="349" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A349" s="5">
         <v>43405</v>
       </c>
@@ -11894,8 +12292,15 @@
         <f t="shared" si="11"/>
         <v>-4.0192182217212409</v>
       </c>
-    </row>
-    <row r="350" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G349" s="5">
+        <v>39508</v>
+      </c>
+      <c r="H349">
+        <f t="shared" si="12"/>
+        <v>-4.0192182217212409</v>
+      </c>
+    </row>
+    <row r="350" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A350" s="5">
         <v>43435</v>
       </c>
@@ -11910,8 +12315,15 @@
         <f t="shared" si="11"/>
         <v>-3.8327553781572945</v>
       </c>
-    </row>
-    <row r="351" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G350" s="5">
+        <v>39539</v>
+      </c>
+      <c r="H350">
+        <f t="shared" si="12"/>
+        <v>-3.8327553781572945</v>
+      </c>
+    </row>
+    <row r="351" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A351" s="5">
         <v>43466</v>
       </c>
@@ -11926,8 +12338,15 @@
         <f t="shared" si="11"/>
         <v>2.28791599829633</v>
       </c>
-    </row>
-    <row r="352" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G351" s="5">
+        <v>39569</v>
+      </c>
+      <c r="H351">
+        <f t="shared" si="12"/>
+        <v>2.28791599829633</v>
+      </c>
+    </row>
+    <row r="352" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A352" s="5">
         <v>43497</v>
       </c>
@@ -11942,8 +12361,15 @@
         <f t="shared" si="11"/>
         <v>5.0724637681160436</v>
       </c>
-    </row>
-    <row r="353" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G352" s="5">
+        <v>39600</v>
+      </c>
+      <c r="H352">
+        <f t="shared" si="12"/>
+        <v>5.0724637681160436</v>
+      </c>
+    </row>
+    <row r="353" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A353" s="5">
         <v>43525</v>
       </c>
@@ -11958,8 +12384,15 @@
         <f t="shared" si="11"/>
         <v>6.769630028167172</v>
       </c>
-    </row>
-    <row r="354" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G353" s="5">
+        <v>39630</v>
+      </c>
+      <c r="H353">
+        <f t="shared" si="12"/>
+        <v>6.769630028167172</v>
+      </c>
+    </row>
+    <row r="354" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A354" s="5">
         <v>43556</v>
       </c>
@@ -11974,8 +12407,15 @@
         <f t="shared" si="11"/>
         <v>6.354001935468661</v>
       </c>
-    </row>
-    <row r="355" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G354" s="5">
+        <v>39661</v>
+      </c>
+      <c r="H354">
+        <f t="shared" si="12"/>
+        <v>6.354001935468661</v>
+      </c>
+    </row>
+    <row r="355" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A355" s="5">
         <v>43586</v>
       </c>
@@ -11990,8 +12430,15 @@
         <f t="shared" si="11"/>
         <v>2.554510307261177</v>
       </c>
-    </row>
-    <row r="356" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G355" s="5">
+        <v>39692</v>
+      </c>
+      <c r="H355">
+        <f t="shared" si="12"/>
+        <v>2.554510307261177</v>
+      </c>
+    </row>
+    <row r="356" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A356" s="5">
         <v>43617</v>
       </c>
@@ -12006,8 +12453,15 @@
         <f t="shared" si="11"/>
         <v>0.23897661777792853</v>
       </c>
-    </row>
-    <row r="357" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G356" s="5">
+        <v>39722</v>
+      </c>
+      <c r="H356">
+        <f t="shared" si="12"/>
+        <v>0.23897661777792853</v>
+      </c>
+    </row>
+    <row r="357" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A357" s="5">
         <v>43647</v>
       </c>
@@ -12022,8 +12476,15 @@
         <f t="shared" si="11"/>
         <v>2.0051299469439527</v>
       </c>
-    </row>
-    <row r="358" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G357" s="5">
+        <v>39753</v>
+      </c>
+      <c r="H357">
+        <f t="shared" si="12"/>
+        <v>2.0051299469439527</v>
+      </c>
+    </row>
+    <row r="358" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A358" s="5">
         <v>43678</v>
       </c>
@@ -12038,8 +12499,15 @@
         <f t="shared" si="11"/>
         <v>-6.0801883299517009E-2</v>
       </c>
-    </row>
-    <row r="359" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G358" s="5">
+        <v>39783</v>
+      </c>
+      <c r="H358">
+        <f t="shared" si="12"/>
+        <v>-6.0801883299517009E-2</v>
+      </c>
+    </row>
+    <row r="359" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A359" s="5">
         <v>43709</v>
       </c>
@@ -12054,8 +12522,15 @@
         <f t="shared" si="11"/>
         <v>0.94013829231606971</v>
       </c>
-    </row>
-    <row r="360" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G359" s="5">
+        <v>39814</v>
+      </c>
+      <c r="H359">
+        <f t="shared" si="12"/>
+        <v>0.94013829231606971</v>
+      </c>
+    </row>
+    <row r="360" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A360" s="5">
         <v>43739</v>
       </c>
@@ -12070,8 +12545,15 @@
         <f t="shared" si="11"/>
         <v>2.7434286626758433</v>
       </c>
-    </row>
-    <row r="361" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G360" s="5">
+        <v>39845</v>
+      </c>
+      <c r="H360">
+        <f t="shared" si="12"/>
+        <v>2.7434286626758433</v>
+      </c>
+    </row>
+    <row r="361" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A361" s="5">
         <v>43770</v>
       </c>
@@ -12086,8 +12568,15 @@
         <f t="shared" si="11"/>
         <v>-0.64349164160302541</v>
       </c>
-    </row>
-    <row r="362" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G361" s="5">
+        <v>39873</v>
+      </c>
+      <c r="H361">
+        <f t="shared" si="12"/>
+        <v>-0.64349164160302541</v>
+      </c>
+    </row>
+    <row r="362" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A362" s="5">
         <v>43800</v>
       </c>
@@ -12102,8 +12591,15 @@
         <f t="shared" si="11"/>
         <v>-1.0917234300645575</v>
       </c>
-    </row>
-    <row r="363" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G362" s="5">
+        <v>39904</v>
+      </c>
+      <c r="H362">
+        <f t="shared" si="12"/>
+        <v>-1.0917234300645575</v>
+      </c>
+    </row>
+    <row r="363" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A363" s="5">
         <v>43831</v>
       </c>
@@ -12118,8 +12614,15 @@
         <f t="shared" si="11"/>
         <v>4.6557239253777301</v>
       </c>
-    </row>
-    <row r="364" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G363" s="5">
+        <v>39934</v>
+      </c>
+      <c r="H363">
+        <f t="shared" si="12"/>
+        <v>4.6557239253777301</v>
+      </c>
+    </row>
+    <row r="364" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A364" s="5">
         <v>43862</v>
       </c>
@@ -12134,8 +12637,15 @@
         <f t="shared" si="11"/>
         <v>3.2887417577944511</v>
       </c>
-    </row>
-    <row r="365" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G364" s="5">
+        <v>39965</v>
+      </c>
+      <c r="H364">
+        <f t="shared" si="12"/>
+        <v>3.2887417577944511</v>
+      </c>
+    </row>
+    <row r="365" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A365" s="5">
         <v>43891</v>
       </c>
@@ -12151,7 +12661,7 @@
         <v>-2.611741238141573</v>
       </c>
     </row>
-    <row r="366" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A366" s="5">
         <v>43922</v>
       </c>
@@ -12167,7 +12677,7 @@
         <v>-8.0243302403967185</v>
       </c>
     </row>
-    <row r="367" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A367" s="5">
         <v>43952</v>
       </c>
@@ -12183,7 +12693,7 @@
         <v>2.3401940020806439E-2</v>
       </c>
     </row>
-    <row r="368" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A368" s="5">
         <v>43983</v>
       </c>
@@ -12527,11 +13037,11 @@
         <v>287.50400000000002</v>
       </c>
       <c r="C389">
-        <f t="shared" ref="C389:C403" si="12">(($B389-$B388)/$B388)*100</f>
+        <f t="shared" ref="C389:C403" si="13">(($B389-$B388)/$B388)*100</f>
         <v>1.3351379548562685</v>
       </c>
       <c r="D389">
-        <f t="shared" ref="D389:D403" si="13">$C389*12</f>
+        <f t="shared" ref="D389:D403" si="14">$C389*12</f>
         <v>16.021655458275223</v>
       </c>
     </row>
@@ -12543,11 +13053,11 @@
         <v>289.10899999999998</v>
       </c>
       <c r="C390">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.55825310256551597</v>
       </c>
       <c r="D390">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>6.6990372307861916</v>
       </c>
     </row>
@@ -12559,11 +13069,11 @@
         <v>292.29599999999999</v>
       </c>
       <c r="C391">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.1023523999598808</v>
       </c>
       <c r="D391">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>13.228228799518568</v>
       </c>
     </row>
@@ -12575,11 +13085,11 @@
         <v>296.31099999999998</v>
       </c>
       <c r="C392">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.3736075758819779</v>
       </c>
       <c r="D392">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>16.483290910583733</v>
       </c>
     </row>
@@ -12591,11 +13101,11 @@
         <v>296.27600000000001</v>
       </c>
       <c r="C393">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>-1.1811913833765257E-2</v>
       </c>
       <c r="D393">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-0.14174296600518307</v>
       </c>
     </row>
@@ -12607,11 +13117,11 @@
         <v>296.17099999999999</v>
       </c>
       <c r="C394">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>-3.5439927635049141E-2</v>
       </c>
       <c r="D394">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-0.42527913162058972</v>
       </c>
     </row>
@@ -12623,11 +13133,11 @@
         <v>296.80799999999999</v>
       </c>
       <c r="C395">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.2150784513000937</v>
       </c>
       <c r="D395">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2.5809414156011243</v>
       </c>
     </row>
@@ -12639,11 +13149,11 @@
         <v>298.012</v>
       </c>
       <c r="C396">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.40564944341123144</v>
       </c>
       <c r="D396">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>4.8677933209347772</v>
       </c>
     </row>
@@ -12655,11 +13165,11 @@
         <v>297.71100000000001</v>
       </c>
       <c r="C397">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>-0.10100264418882049</v>
       </c>
       <c r="D397">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-1.2120317302658459</v>
       </c>
     </row>
@@ -12671,11 +13181,11 @@
         <v>296.79700000000003</v>
       </c>
       <c r="C398">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>-0.30700914645410721</v>
       </c>
       <c r="D398">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-3.6841097574492867</v>
       </c>
     </row>
@@ -12687,11 +13197,11 @@
         <v>299.17</v>
       </c>
       <c r="C399">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.79953638345400746</v>
       </c>
       <c r="D399">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>9.5944366014480895</v>
       </c>
     </row>
@@ -12703,11 +13213,11 @@
         <v>300.83999999999997</v>
       </c>
       <c r="C400">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.55821105057323894</v>
       </c>
       <c r="D400">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>6.6985326068788673</v>
       </c>
     </row>
@@ -12719,11 +13229,11 @@
         <v>301.83600000000001</v>
       </c>
       <c r="C401">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.33107299561229819</v>
       </c>
       <c r="D401">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3.9728759473475783</v>
       </c>
     </row>
@@ -12735,11 +13245,11 @@
         <v>303.363</v>
       </c>
       <c r="C402">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.50590386832584144</v>
       </c>
       <c r="D402">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>6.0708464199100973</v>
       </c>
     </row>
@@ -12751,11 +13261,11 @@
         <v>304.12700000000001</v>
       </c>
       <c r="C403">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.25184350102023317</v>
       </c>
       <c r="D403">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3.0221220122427983</v>
       </c>
     </row>

</xml_diff>